<commit_message>
Add new tool to generate dates and ics files
</commit_message>
<xml_diff>
--- a/termine/termine.xlsx
+++ b/termine/termine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Projects/private/dorfhaexe-app/termine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AC6976-00C9-4541-9857-B6758D943014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475DEB01-8BE3-6049-BBD2-423A387DB451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29100" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29100" windowHeight="17820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Narrenfahrplan" sheetId="1" r:id="rId1"/>
@@ -339,8 +339,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="168" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -568,34 +568,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -941,7 +941,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AAE740-EBED-C44F-88CC-3EA9570BD07B}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>